<commit_message>
refactor: realizar correcciones y mejoras de formato en el notebook para mayor claridad
</commit_message>
<xml_diff>
--- a/data/alertas_generadas.xlsx
+++ b/data/alertas_generadas.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,24 +440,24 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
+        <v>4</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Supermercados Rey</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
         <v>1</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Supermercados Rey</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Embonor</t>
+          <t>Supermercados Rey</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -466,7 +466,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -474,32 +474,19 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Supermercados Rey</t>
+          <t>Embonor</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>8</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Cruz Verde</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
         <v>3</v>
       </c>
     </row>

</xml_diff>